<commit_message>
calibrated dynamic model running
</commit_message>
<xml_diff>
--- a/Firm_Parameters_FullertonRogers.xlsx
+++ b/Firm_Parameters_FullertonRogers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="xi" sheetId="1" r:id="rId1"/>
@@ -147,8 +147,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -217,7 +227,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -246,6 +256,11 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -274,6 +289,11 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -1872,7 +1892,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3018,15 +3038,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3034,159 +3054,216 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3204,15 +3281,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3220,159 +3297,216 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -3390,15 +3524,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3406,159 +3540,216 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.67589999999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.7117</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0.90249999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.90329999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.78300000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10">
         <v>0.96030000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0.9123</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.73729999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0.81589999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14">
         <v>0.92279999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.79490000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -3576,15 +3767,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3592,143 +3783,211 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.1565</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <f>1/17</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2.93E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <f t="shared" ref="C3:C18" si="0">1/17</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>4.0599999999999997E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.14480000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>2.3900000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2.5700000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.11409999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>2.93E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>8.6900000000000005E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.1595</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>3.9600000000000003E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>5.33E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>9.4999999999999998E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>3.4099999999999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>2.7300000000000001E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>1.9699999999999999E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>8</v>
       </c>

</xml_diff>